<commit_message>
Fixes #25 all the errors generated are in the proper range Fixes #24 The file Dialog is in a subVI, it is used in all the places a file is open so its the only place that contains the file extension. Added tag #USERCFG  so users know to configure this. Fixes #22 The only location for dialogs is in the error case and the File Dialog Vi
</commit_message>
<xml_diff>
--- a/Documentation/Errors.xlsx
+++ b/Documentation/Errors.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Error Code</t>
   </si>
@@ -28,6 +28,21 @@
   </si>
   <si>
     <t>Range 538500 to 550</t>
+  </si>
+  <si>
+    <t>Glyph not found</t>
+  </si>
+  <si>
+    <t>Non Message Handelr for the message</t>
+  </si>
+  <si>
+    <t>Unknown item command:  for custome menu</t>
+  </si>
+  <si>
+    <t>Unknown Menu Option for Application Menu</t>
+  </si>
+  <si>
+    <t>Unsupported Config Version</t>
   </si>
 </sst>
 </file>
@@ -359,16 +374,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -388,6 +403,126 @@
     <row r="2" spans="1:4">
       <c r="A2">
         <v>538500</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3">
+        <v>538501</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4">
+        <v>538502</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5">
+        <v>538503</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6">
+        <v>538504</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7">
+        <v>538505</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8">
+        <v>538506</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9">
+        <v>538507</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10">
+        <v>538508</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11">
+        <v>538509</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12">
+        <v>538510</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13">
+        <v>538511</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14">
+        <v>538512</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15">
+        <v>538513</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16">
+        <v>538514</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17">
+        <v>538515</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18">
+        <v>538516</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19">
+        <v>538517</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20">
+        <v>538518</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21">
+        <v>538519</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22">
+        <v>538520</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23">
+        <v>538521</v>
       </c>
     </row>
   </sheetData>

</xml_diff>